<commit_message>
Publish WECC unit commitment data set and correct hydro for WECC expansion
12 zone WECC test system for unit commitment/economic dispatch projects

Update to WECC expansion data including reservoir capacity (MWh) for hydro resources.
</commit_message>
<xml_diff>
--- a/Project/wecc_2045_all_clean_expansion/Input_descriptions_WECC_expansion.xlsx
+++ b/Project/wecc_2045_all_clean_expansion/Input_descriptions_WECC_expansion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdj2/Dropbox (Princeton)/Princeton/02 - Energy Systems Modeling Course/Test systems/wecc_2045_all_clean_expansion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdj2/power-systems-optimization/Project/wecc_2045_all_clean_expansion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C508015-E1A0-3A47-BAD3-0EC04317CF7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06F3796-FA64-8F49-8BD2-D63A7858F46E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29600" yWindow="-2320" windowWidth="28800" windowHeight="17540" activeTab="9" xr2:uid="{E2F8FAF9-854F-D04B-BF15-2CC6D544468C}"/>
+    <workbookView xWindow="-29600" yWindow="-2320" windowWidth="28800" windowHeight="17540" xr2:uid="{E2F8FAF9-854F-D04B-BF15-2CC6D544468C}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="8" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="179">
   <si>
     <t>R_ID</t>
   </si>
@@ -614,6 +614,9 @@
   </si>
   <si>
     <t>Hourly avaialbility factor (maximum hourly load by type as p.u. share of maximum instanataneous demand reported in Flexible_load_data.csv)</t>
+  </si>
+  <si>
+    <t>Transmission transfer limits from EPA IPM model</t>
   </si>
 </sst>
 </file>
@@ -1011,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C32E7C-8FDE-6A41-B615-89F1843867D7}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1060,6 +1063,11 @@
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="3" t="s">
         <v>165</v>
       </c>
     </row>
@@ -1072,7 +1080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD3AD30-E935-1D4B-BC2F-6EA444FF2658}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>